<commit_message>
ajuste informations temps/agents requis
</commit_message>
<xml_diff>
--- a/inst/extdata/fiche.xlsx
+++ b/inst/extdata/fiche.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\R\FichesSRC\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B1C193-0492-46BA-8ACF-775DDD19D5C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F6A32E-6FC9-40CD-893B-D4F81AE25F47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{98796B84-567B-45ED-BADB-C7585C647EFF}"/>
   </bookViews>
@@ -376,84 +376,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -461,6 +383,60 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -479,14 +455,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -506,14 +497,23 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,19 +587,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>721180</xdr:colOff>
+      <xdr:colOff>722133</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>13608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1118728</xdr:colOff>
+      <xdr:colOff>1117775</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>164321</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 2" descr="C:\Users\mila.betemps\Desktop\Fiches de réseaux de suivi\66403.png">
+        <xdr:cNvPr id="5" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380664B7-4844-41A7-BBF4-038EAA9C47FF}"/>
@@ -618,15 +618,14 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7361466" y="979715"/>
-          <a:ext cx="397548" cy="395642"/>
+          <a:off x="7648169" y="966108"/>
+          <a:ext cx="395642" cy="395642"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -647,20 +646,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>299357</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>40821</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>748395</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>143691</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>41652</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>68868</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>111320</xdr:rowOff>
+      <xdr:rowOff>8450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 2" descr="C:\Users\mila.betemps\Desktop\Fiches de réseaux de suivi\Image bonhomme.png">
+        <xdr:cNvPr id="6" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C68EE5CF-E0E7-47E7-AAE8-3D51D127ADC2}"/>
@@ -679,15 +678,14 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10355036" y="1006928"/>
-          <a:ext cx="504295" cy="519535"/>
+          <a:off x="8858252" y="905691"/>
+          <a:ext cx="504295" cy="504295"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1220,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B58E52B9-9C60-40F0-8AF6-2B7840091574}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47:Q47"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,60 +1242,60 @@
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
@@ -1336,11 +1334,11 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="60" t="s">
+      <c r="O5" s="34" t="s">
         <v>21</v>
       </c>
       <c r="P5" s="4"/>
-      <c r="Q5" s="61"/>
+      <c r="Q5" s="35"/>
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -1352,18 +1350,18 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="5"/>
       <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="61"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="35"/>
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1373,17 +1371,17 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="61"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="35"/>
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1391,12 +1389,12 @@
       <c r="B8" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="78"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="42"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="12"/>
@@ -1405,18 +1403,18 @@
       <c r="N8" s="12"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="61"/>
+      <c r="Q8" s="35"/>
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="27"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="78"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="42"/>
       <c r="I9" s="5"/>
       <c r="J9" s="7"/>
       <c r="K9" s="13" t="s">
@@ -1425,20 +1423,20 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="65"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="57"/>
       <c r="R9" s="31"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="27"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="78"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="42"/>
       <c r="I10" s="5"/>
       <c r="J10" s="7"/>
       <c r="K10" s="20" t="s">
@@ -1447,33 +1445,33 @@
       <c r="L10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="55" t="s">
+      <c r="M10" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="56"/>
-      <c r="O10" s="63"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="65"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="57"/>
       <c r="R10" s="5"/>
     </row>
     <row r="11" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="28"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="78"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="42"/>
       <c r="I11" s="5"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="65"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="57"/>
       <c r="R11" s="5"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1481,74 +1479,74 @@
       <c r="B12" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="80" t="s">
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="79"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="5"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="70"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="63"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="65"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="55"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="57"/>
       <c r="R12" s="5"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="50"/>
       <c r="I13" s="5"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="70"/>
-      <c r="L13" s="70"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="65"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="57"/>
       <c r="R13" s="5"/>
     </row>
     <row r="14" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="27"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="46"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="50"/>
       <c r="I14" s="5"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="66"/>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="68"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="60"/>
       <c r="R14" s="5"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="28"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="46"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="18" t="s">
@@ -1569,123 +1567,123 @@
       <c r="B16" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="50"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="46"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="50"/>
       <c r="R16" s="5"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="27"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="46"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="50"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="46"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="50"/>
       <c r="R17" s="5"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="27"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="46"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="50"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="46"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="50"/>
       <c r="R18" s="5"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="46"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="50"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="46"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="50"/>
       <c r="R19" s="5"/>
     </row>
     <row r="20" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="28"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="46"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="50"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="46"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="50"/>
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
       <c r="F21" s="14"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="46"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="50"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="46"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="53"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="50"/>
       <c r="R21" s="5"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1693,19 +1691,19 @@
       <c r="B22" s="15"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="46"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="50"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="47"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="46"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="53"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="50"/>
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1713,19 +1711,19 @@
       <c r="B23" s="15"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="46"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="50"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="46"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="50"/>
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1733,19 +1731,19 @@
       <c r="B24" s="15"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="46"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="50"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="46"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="50"/>
       <c r="R24" s="5"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1753,19 +1751,19 @@
       <c r="B25" s="15"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="50"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="52"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="47"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="46"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="50"/>
       <c r="R25" s="5"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -1773,21 +1771,21 @@
       <c r="B26" s="15"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
       <c r="G26" s="18" t="s">
         <v>6</v>
       </c>
       <c r="H26" s="19"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="46"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="53"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="50"/>
       <c r="R26" s="5"/>
     </row>
     <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1795,19 +1793,19 @@
       <c r="B27" s="15"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="39"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="66"/>
       <c r="G27" s="29"/>
       <c r="H27" s="30"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="50"/>
-      <c r="O27" s="48"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="50"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="54"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="52"/>
       <c r="R27" s="5"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -1815,10 +1813,10 @@
       <c r="B28" s="15"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="46"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="50"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="25" t="s">
@@ -1837,19 +1835,19 @@
       <c r="B29" s="15"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="46"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="50"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="72"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="73"/>
-      <c r="N29" s="73"/>
-      <c r="O29" s="73"/>
-      <c r="P29" s="73"/>
-      <c r="Q29" s="74"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="70"/>
+      <c r="M29" s="70"/>
+      <c r="N29" s="70"/>
+      <c r="O29" s="70"/>
+      <c r="P29" s="70"/>
+      <c r="Q29" s="71"/>
       <c r="R29" s="5"/>
     </row>
     <row r="30" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1857,19 +1855,19 @@
       <c r="B30" s="15"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="46"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="50"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="76"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="76"/>
-      <c r="P30" s="76"/>
-      <c r="Q30" s="77"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="73"/>
+      <c r="M30" s="73"/>
+      <c r="N30" s="73"/>
+      <c r="O30" s="73"/>
+      <c r="P30" s="73"/>
+      <c r="Q30" s="74"/>
       <c r="R30" s="5"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -1877,10 +1875,10 @@
       <c r="B31" s="15"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="46"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="50"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="18" t="s">
@@ -1901,10 +1899,10 @@
       <c r="B32" s="15"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="46"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="50"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="8"/>
@@ -1921,19 +1919,19 @@
       <c r="B33" s="15"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="46"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="50"/>
       <c r="I33" s="5"/>
       <c r="J33" s="4"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="47"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="46"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="53"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="50"/>
       <c r="R33" s="5"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -1941,19 +1939,19 @@
       <c r="B34" s="15"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="46"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="50"/>
       <c r="I34" s="5"/>
       <c r="J34" s="4"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="46"/>
-      <c r="O34" s="47"/>
-      <c r="P34" s="45"/>
-      <c r="Q34" s="46"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="53"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="50"/>
       <c r="R34" s="5"/>
     </row>
     <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1961,28 +1959,28 @@
       <c r="B35" s="16"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="50"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="52"/>
       <c r="I35" s="5"/>
       <c r="J35" s="4"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="46"/>
-      <c r="O35" s="47"/>
-      <c r="P35" s="45"/>
-      <c r="Q35" s="46"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="53"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="50"/>
       <c r="R35" s="5"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="18" t="s">
@@ -1992,212 +1990,212 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="8"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="46"/>
-      <c r="O36" s="47"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="53"/>
+      <c r="P36" s="49"/>
+      <c r="Q36" s="50"/>
       <c r="R36" s="5"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="77"/>
       <c r="G37" s="29"/>
       <c r="H37" s="30"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="8"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="47"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="46"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="53"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="50"/>
       <c r="R37" s="5"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="46"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="50"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="8"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="46"/>
-      <c r="O38" s="47"/>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="46"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="53"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="50"/>
       <c r="R38" s="5"/>
     </row>
     <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="46"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="50"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="8"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="46"/>
-      <c r="O39" s="47"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="46"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="50"/>
       <c r="R39" s="5"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="46"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="50"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="8"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="45"/>
-      <c r="N40" s="46"/>
-      <c r="O40" s="47"/>
-      <c r="P40" s="45"/>
-      <c r="Q40" s="46"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="50"/>
       <c r="R40" s="5"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="46"/>
+      <c r="B41" s="75"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="50"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="46"/>
-      <c r="O41" s="47"/>
-      <c r="P41" s="45"/>
-      <c r="Q41" s="46"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="50"/>
       <c r="R41" s="5"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="46"/>
+      <c r="B42" s="75"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="50"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="8"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="46"/>
-      <c r="O42" s="47"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="50"/>
       <c r="R42" s="5"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="46"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="50"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="8"/>
-      <c r="L43" s="45"/>
-      <c r="M43" s="45"/>
-      <c r="N43" s="46"/>
-      <c r="O43" s="47"/>
-      <c r="P43" s="45"/>
-      <c r="Q43" s="46"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="49"/>
+      <c r="Q43" s="50"/>
       <c r="R43" s="5"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="46"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="50"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="8"/>
-      <c r="L44" s="45"/>
-      <c r="M44" s="45"/>
-      <c r="N44" s="46"/>
-      <c r="O44" s="47"/>
-      <c r="P44" s="45"/>
-      <c r="Q44" s="46"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="50"/>
       <c r="R44" s="5"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="46"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="66"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="50"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="8"/>
-      <c r="L45" s="45"/>
-      <c r="M45" s="45"/>
-      <c r="N45" s="46"/>
-      <c r="O45" s="47"/>
-      <c r="P45" s="45"/>
-      <c r="Q45" s="46"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="53"/>
+      <c r="P45" s="49"/>
+      <c r="Q45" s="50"/>
       <c r="R45" s="5"/>
     </row>
     <row r="46" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="50"/>
+      <c r="B46" s="79"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="52"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="9"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
       <c r="N46" s="10"/>
-      <c r="O46" s="48"/>
-      <c r="P46" s="49"/>
-      <c r="Q46" s="50"/>
+      <c r="O46" s="54"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="52"/>
       <c r="R46" s="5"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -2205,43 +2203,43 @@
         <v>18</v>
       </c>
       <c r="B47" s="2"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="63"/>
       <c r="I47" s="2"/>
       <c r="J47" s="24" t="s">
         <v>18</v>
       </c>
       <c r="K47" s="2"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-      <c r="N47" s="43"/>
-      <c r="O47" s="43"/>
-      <c r="P47" s="43"/>
-      <c r="Q47" s="43"/>
+      <c r="L47" s="63"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="63"/>
+      <c r="O47" s="63"/>
+      <c r="P47" s="63"/>
+      <c r="Q47" s="63"/>
       <c r="R47" s="32"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="80"/>
+      <c r="G48" s="80"/>
+      <c r="H48" s="80"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="69"/>
-      <c r="M48" s="69"/>
-      <c r="N48" s="69"/>
-      <c r="O48" s="69"/>
-      <c r="P48" s="69"/>
-      <c r="Q48" s="69"/>
+      <c r="L48" s="64"/>
+      <c r="M48" s="64"/>
+      <c r="N48" s="64"/>
+      <c r="O48" s="64"/>
+      <c r="P48" s="64"/>
+      <c r="Q48" s="64"/>
       <c r="R48" s="32"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -2249,30 +2247,43 @@
         <v>19</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="69"/>
-      <c r="D49" s="69"/>
-      <c r="E49" s="69"/>
-      <c r="F49" s="69"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="69"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="L49" s="69"/>
-      <c r="M49" s="69"/>
-      <c r="N49" s="69"/>
-      <c r="O49" s="69"/>
-      <c r="P49" s="69"/>
-      <c r="Q49" s="69"/>
+      <c r="L49" s="64"/>
+      <c r="M49" s="64"/>
+      <c r="N49" s="64"/>
+      <c r="O49" s="64"/>
+      <c r="P49" s="64"/>
+      <c r="Q49" s="64"/>
       <c r="R49" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
+    <mergeCell ref="K16:N27"/>
     <mergeCell ref="L47:Q47"/>
     <mergeCell ref="L48:Q48"/>
     <mergeCell ref="L49:Q49"/>
     <mergeCell ref="E22:F35"/>
     <mergeCell ref="G13:H25"/>
+    <mergeCell ref="O16:Q27"/>
+    <mergeCell ref="K29:Q30"/>
+    <mergeCell ref="L33:N45"/>
+    <mergeCell ref="O33:Q46"/>
+    <mergeCell ref="B37:F42"/>
+    <mergeCell ref="B43:F46"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="C49:H49"/>
+    <mergeCell ref="G38:H46"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:N7"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="G6:H11"/>
     <mergeCell ref="L1:P3"/>
@@ -2283,22 +2294,10 @@
     <mergeCell ref="C12:F15"/>
     <mergeCell ref="C16:F20"/>
     <mergeCell ref="G28:H35"/>
-    <mergeCell ref="L6:M7"/>
     <mergeCell ref="O9:Q14"/>
     <mergeCell ref="K11:K14"/>
     <mergeCell ref="L11:L14"/>
     <mergeCell ref="M11:N14"/>
-    <mergeCell ref="K16:N27"/>
-    <mergeCell ref="O16:Q27"/>
-    <mergeCell ref="K29:Q30"/>
-    <mergeCell ref="L33:N45"/>
-    <mergeCell ref="O33:Q46"/>
-    <mergeCell ref="B37:F42"/>
-    <mergeCell ref="B43:F46"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="C48:H48"/>
-    <mergeCell ref="C49:H49"/>
-    <mergeCell ref="G38:H46"/>
   </mergeCells>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="7.874015748031496E-2" bottom="7.874015748031496E-2" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajuste le format de la fiche papier
</commit_message>
<xml_diff>
--- a/inst/extdata/fiche.xlsx
+++ b/inst/extdata/fiche.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\R\FichesSRC\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F6A32E-6FC9-40CD-893B-D4F81AE25F47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DDF65F-0B60-4AA7-AAE1-51FD0009893C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{98796B84-567B-45ED-BADB-C7585C647EFF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Description</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Partenariats</t>
-  </si>
-  <si>
-    <t>Transversalité</t>
   </si>
   <si>
     <t>Logistique</t>
@@ -78,9 +75,6 @@
     <t>Saisie/Validation des données</t>
   </si>
   <si>
-    <t>Autres relevés</t>
-  </si>
-  <si>
     <t>En savoir plus</t>
   </si>
   <si>
@@ -92,12 +86,15 @@
   <si>
     <t>Compétences</t>
   </si>
+  <si>
+    <t>Autres informations</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,12 +136,6 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Marianne"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
@@ -152,19 +143,8 @@
       <family val="3"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Marianne"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Marianne"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Marianne"/>
       <family val="3"/>
     </font>
@@ -189,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -323,11 +303,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -337,8 +386,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -352,10 +399,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -363,32 +407,48 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -410,110 +470,107 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,7 +652,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>1117775</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>164321</xdr:rowOff>
+      <xdr:rowOff>164322</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -654,8 +711,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>68868</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>8450</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>158129</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -708,14 +765,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>639535</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>68038</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>933029</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>141196</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>113984</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -730,8 +787,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7279821" y="6368143"/>
-          <a:ext cx="293494" cy="2359160"/>
+          <a:off x="7565571" y="6272895"/>
+          <a:ext cx="293494" cy="2549660"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst/>
@@ -1219,7 +1276,7 @@
   <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:N7"/>
+      <selection activeCell="K45" sqref="K45:Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,60 +1299,60 @@
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
@@ -1319,8 +1376,10 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1329,39 +1388,37 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="J5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="35"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="27"/>
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="36"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="35"/>
       <c r="P6" s="36"/>
-      <c r="Q6" s="35"/>
+      <c r="Q6" s="27"/>
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1370,837 +1427,835 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="36"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="35"/>
       <c r="P7" s="36"/>
-      <c r="Q7" s="35"/>
+      <c r="Q7" s="27"/>
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="42"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="45"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="35"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="27"/>
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="42"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="5"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="13" t="s">
-        <v>9</v>
+      <c r="K9" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="31"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="24"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="42"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="45"/>
       <c r="I10" s="5"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="20" t="s">
+      <c r="M10" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="45" t="s">
+      <c r="N10" s="48"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="5"/>
+    </row>
+    <row r="11" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="28"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="5"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="72"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="5"/>
+    </row>
+    <row r="14" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="75"/>
+      <c r="P14" s="76"/>
+      <c r="Q14" s="77"/>
+      <c r="R14" s="5"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="46"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="57"/>
-      <c r="R10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="5"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="37"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="57"/>
-      <c r="R12" s="5"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="18" t="s">
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="18" t="s">
+      <c r="P15" s="19"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="5"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="5"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="67"/>
+      <c r="R17" s="5"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="70"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="5"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="5"/>
+    </row>
+    <row r="20" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="66"/>
+      <c r="M20" s="66"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="70"/>
+      <c r="P20" s="66"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="5"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="70"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="5"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="70"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="5"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="70"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="5"/>
+    </row>
+    <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="70"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="67"/>
+      <c r="R24" s="5"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="66"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="70"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="5"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="66"/>
+      <c r="M26" s="66"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="70"/>
+      <c r="P26" s="66"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="5"/>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="68"/>
+      <c r="N27" s="69"/>
+      <c r="O27" s="71"/>
+      <c r="P27" s="68"/>
+      <c r="Q27" s="69"/>
+      <c r="R27" s="5"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="5"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="53"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="5"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="49"/>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="5"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="53"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="50"/>
-      <c r="R18" s="5"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="5"/>
-    </row>
-    <row r="20" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="5"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="53"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="5"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="53"/>
-      <c r="P22" s="49"/>
-      <c r="Q22" s="50"/>
-      <c r="R22" s="5"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="49"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="5"/>
-    </row>
-    <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="53"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="50"/>
-      <c r="R24" s="5"/>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="53"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="50"/>
-      <c r="R25" s="5"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="18" t="s">
+      <c r="P28" s="19"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="5"/>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="70"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="67"/>
+      <c r="R29" s="5"/>
+    </row>
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="19"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="53"/>
-      <c r="P26" s="49"/>
-      <c r="Q26" s="50"/>
-      <c r="R26" s="5"/>
-    </row>
-    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="54"/>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="52"/>
-      <c r="R27" s="5"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="5"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="70"/>
-      <c r="M29" s="70"/>
-      <c r="N29" s="70"/>
-      <c r="O29" s="70"/>
-      <c r="P29" s="70"/>
-      <c r="Q29" s="71"/>
-      <c r="R29" s="5"/>
-    </row>
-    <row r="30" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="50"/>
+      <c r="H30" s="17"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="72"/>
-      <c r="L30" s="73"/>
-      <c r="M30" s="73"/>
-      <c r="N30" s="73"/>
-      <c r="O30" s="73"/>
-      <c r="P30" s="73"/>
-      <c r="Q30" s="74"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="70"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="67"/>
       <c r="R30" s="5"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="15"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="50"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="38"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="19"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="70"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="67"/>
       <c r="R31" s="5"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="15"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="66"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="50"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="38"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="8"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="7"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="70"/>
+      <c r="P32" s="66"/>
+      <c r="Q32" s="67"/>
       <c r="R32" s="5"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="15"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="50"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="38"/>
       <c r="I33" s="5"/>
       <c r="J33" s="4"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="53"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="50"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="70"/>
+      <c r="P33" s="66"/>
+      <c r="Q33" s="67"/>
       <c r="R33" s="5"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="15"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="66"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="50"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="38"/>
       <c r="I34" s="5"/>
       <c r="J34" s="4"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="53"/>
-      <c r="P34" s="49"/>
-      <c r="Q34" s="50"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="66"/>
+      <c r="Q34" s="67"/>
       <c r="R34" s="5"/>
     </row>
     <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="52"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="38"/>
       <c r="I35" s="5"/>
       <c r="J35" s="4"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="53"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="50"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="70"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="67"/>
       <c r="R35" s="5"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="19"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="38"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="8"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="50"/>
-      <c r="O36" s="53"/>
-      <c r="P36" s="49"/>
-      <c r="Q36" s="50"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="70"/>
+      <c r="P36" s="66"/>
+      <c r="Q36" s="67"/>
       <c r="R36" s="5"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="75"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="30"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="38"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="8"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="50"/>
-      <c r="O37" s="53"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="50"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="70"/>
+      <c r="P37" s="66"/>
+      <c r="Q37" s="67"/>
       <c r="R37" s="5"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="75"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="77"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="50"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="38"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="8"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="50"/>
-      <c r="O38" s="53"/>
-      <c r="P38" s="49"/>
-      <c r="Q38" s="50"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="38"/>
+      <c r="O38" s="70"/>
+      <c r="P38" s="66"/>
+      <c r="Q38" s="67"/>
       <c r="R38" s="5"/>
     </row>
     <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="75"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="50"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="38"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="8"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="53"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="50"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="70"/>
+      <c r="P39" s="66"/>
+      <c r="Q39" s="67"/>
       <c r="R39" s="5"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="75"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="77"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="50"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="38"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="8"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="50"/>
-      <c r="O40" s="53"/>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="50"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="37"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="70"/>
+      <c r="P40" s="66"/>
+      <c r="Q40" s="67"/>
       <c r="R40" s="5"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
-      <c r="B41" s="75"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="77"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="50"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="38"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="50"/>
-      <c r="O41" s="53"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="50"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="70"/>
+      <c r="P41" s="66"/>
+      <c r="Q41" s="67"/>
       <c r="R41" s="5"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="50"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="38"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="50"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="50"/>
+      <c r="K42" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="32"/>
       <c r="R42" s="5"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="78"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="66"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="50"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="38"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="53"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="50"/>
+      <c r="K43" s="78"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="66"/>
+      <c r="O43" s="66"/>
+      <c r="P43" s="66"/>
+      <c r="Q43" s="79"/>
       <c r="R43" s="5"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="78"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="50"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="38"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="53"/>
-      <c r="P44" s="49"/>
-      <c r="Q44" s="50"/>
+      <c r="K44" s="78"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="66"/>
+      <c r="O44" s="66"/>
+      <c r="P44" s="66"/>
+      <c r="Q44" s="79"/>
       <c r="R44" s="5"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
-      <c r="F45" s="66"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="50"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="38"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="49"/>
-      <c r="M45" s="49"/>
-      <c r="N45" s="50"/>
-      <c r="O45" s="53"/>
-      <c r="P45" s="49"/>
-      <c r="Q45" s="50"/>
+      <c r="K45" s="78"/>
+      <c r="L45" s="66"/>
+      <c r="M45" s="66"/>
+      <c r="N45" s="66"/>
+      <c r="O45" s="66"/>
+      <c r="P45" s="66"/>
+      <c r="Q45" s="79"/>
       <c r="R45" s="5"/>
     </row>
     <row r="46" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
-      <c r="B46" s="79"/>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="68"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="52"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="41"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="54"/>
-      <c r="P46" s="51"/>
-      <c r="Q46" s="52"/>
+      <c r="K46" s="80"/>
+      <c r="L46" s="81"/>
+      <c r="M46" s="81"/>
+      <c r="N46" s="81"/>
+      <c r="O46" s="81"/>
+      <c r="P46" s="81"/>
+      <c r="Q46" s="82"/>
       <c r="R46" s="5"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
-        <v>18</v>
+      <c r="A47" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="63"/>
@@ -2210,78 +2265,72 @@
       <c r="G47" s="63"/>
       <c r="H47" s="63"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="24" t="s">
-        <v>18</v>
+      <c r="J47" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="K47" s="2"/>
-      <c r="L47" s="63"/>
-      <c r="M47" s="63"/>
-      <c r="N47" s="63"/>
-      <c r="O47" s="63"/>
-      <c r="P47" s="63"/>
-      <c r="Q47" s="63"/>
-      <c r="R47" s="32"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="52"/>
+      <c r="P47" s="52"/>
+      <c r="Q47" s="52"/>
+      <c r="R47" s="25"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="80"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="80"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="64"/>
-      <c r="M48" s="64"/>
-      <c r="N48" s="64"/>
-      <c r="O48" s="64"/>
-      <c r="P48" s="64"/>
-      <c r="Q48" s="64"/>
-      <c r="R48" s="32"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="53"/>
+      <c r="N48" s="53"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="25"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
-        <v>19</v>
+      <c r="A49" s="26" t="s">
+        <v>17</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="L49" s="64"/>
-      <c r="M49" s="64"/>
-      <c r="N49" s="64"/>
-      <c r="O49" s="64"/>
-      <c r="P49" s="64"/>
-      <c r="Q49" s="64"/>
-      <c r="R49" s="32"/>
+      <c r="L49" s="53"/>
+      <c r="M49" s="53"/>
+      <c r="N49" s="53"/>
+      <c r="O49" s="53"/>
+      <c r="P49" s="53"/>
+      <c r="Q49" s="53"/>
+      <c r="R49" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="K16:N27"/>
     <mergeCell ref="L47:Q47"/>
     <mergeCell ref="L48:Q48"/>
     <mergeCell ref="L49:Q49"/>
     <mergeCell ref="E22:F35"/>
-    <mergeCell ref="G13:H25"/>
     <mergeCell ref="O16:Q27"/>
-    <mergeCell ref="K29:Q30"/>
-    <mergeCell ref="L33:N45"/>
-    <mergeCell ref="O33:Q46"/>
     <mergeCell ref="B37:F42"/>
     <mergeCell ref="B43:F46"/>
     <mergeCell ref="C47:H47"/>
     <mergeCell ref="C48:H48"/>
     <mergeCell ref="C49:H49"/>
-    <mergeCell ref="G38:H46"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:N7"/>
     <mergeCell ref="B36:D36"/>
@@ -2293,11 +2342,17 @@
     <mergeCell ref="C8:F11"/>
     <mergeCell ref="C12:F15"/>
     <mergeCell ref="C16:F20"/>
-    <mergeCell ref="G28:H35"/>
     <mergeCell ref="O9:Q14"/>
     <mergeCell ref="K11:K14"/>
     <mergeCell ref="L11:L14"/>
     <mergeCell ref="M11:N14"/>
+    <mergeCell ref="K16:N27"/>
+    <mergeCell ref="K45:Q46"/>
+    <mergeCell ref="L29:N41"/>
+    <mergeCell ref="O29:Q41"/>
+    <mergeCell ref="K43:Q44"/>
+    <mergeCell ref="G13:H29"/>
+    <mergeCell ref="G31:H46"/>
   </mergeCells>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="7.874015748031496E-2" bottom="7.874015748031496E-2" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>